<commit_message>
Lithium Ion AA Batteries - Initial 4 brands testing completed
</commit_message>
<xml_diff>
--- a/hardware/battery-capacity-tests_lithium-ion_AA-AAA.xlsx
+++ b/hardware/battery-capacity-tests_lithium-ion_AA-AAA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcava\Documents\GitHub\Coding\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC3720-F744-48CB-B756-CC772F8FD6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79868D48-6006-4AA6-B38C-B9DE75A12C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E5D7BF72-F0C5-4096-89C0-8DC37475FB76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="23">
   <si>
     <t>Brand</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Battery #</t>
-  </si>
-  <si>
     <t>Cutoff</t>
   </si>
   <si>
@@ -75,6 +72,39 @@
   </si>
   <si>
     <t>AAA</t>
+  </si>
+  <si>
+    <t>Batt #</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>KILISTEELS</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Plug Loc</t>
+  </si>
+  <si>
+    <t>USB Type</t>
+  </si>
+  <si>
+    <t>USB C</t>
+  </si>
+  <si>
+    <t>MICRO</t>
+  </si>
+  <si>
+    <t>SIDE</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>0.35 A</t>
   </si>
 </sst>
 </file>
@@ -83,9 +113,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,###&quot; V&quot;"/>
-    <numFmt numFmtId="166" formatCode="0&quot; mAh&quot;"/>
+    <numFmt numFmtId="165" formatCode="0&quot; mAh&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +128,29 @@
       <color theme="1"/>
       <name val="Fira Code"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Fira Code"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Fira Code"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -134,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -143,20 +189,50 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -168,12 +244,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="166" formatCode="0&quot; mAh&quot;"/>
+      <numFmt numFmtId="165" formatCode="0&quot; mAh&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="dotted">
           <color indexed="64"/>
@@ -206,12 +282,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,###&quot; V&quot;"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="dotted">
@@ -245,11 +321,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,###&quot; V&quot;"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="dotted">
@@ -283,11 +360,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="dotted">
           <color indexed="64"/>
@@ -320,7 +398,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
@@ -357,11 +435,31 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="dotted">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -374,7 +472,99 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Fira Code"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="dotted">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Fira Code"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="dotted">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Fira Code"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Fira Code"/>
         <scheme val="none"/>
@@ -394,16 +584,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90FDC6D0-C24B-4FCF-97E3-42B850F8B680}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E29" xr:uid="{90FDC6D0-C24B-4FCF-97E3-42B850F8B680}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
-    <sortCondition ref="A1:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90FDC6D0-C24B-4FCF-97E3-42B850F8B680}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+  <autoFilter ref="A1:H33" xr:uid="{90FDC6D0-C24B-4FCF-97E3-42B850F8B680}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
+    <sortCondition ref="B1:B33"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E621E886-FF19-4F2A-9DC2-BE55D0D49A62}" name="Brand" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{970D62AB-2D93-4B0E-AF18-58B89109CB56}" name="Size" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BEBCCB39-C2AB-4780-9A7C-EA8AF608ACDD}" name="Battery #" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{91078071-EBF5-4F85-928F-09C02DDAA78B}" name="Cutoff" dataDxfId="1"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{E621E886-FF19-4F2A-9DC2-BE55D0D49A62}" name="Brand" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{970D62AB-2D93-4B0E-AF18-58B89109CB56}" name="Size" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{2D695DFE-BB2F-4898-8193-3E441333E394}" name="USB Type" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C4ED642C-3E83-407A-B615-71CDCD59B8BB}" name="Plug Loc" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BEBCCB39-C2AB-4780-9A7C-EA8AF608ACDD}" name="Batt #" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{91078071-EBF5-4F85-928F-09C02DDAA78B}" name="Cutoff" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{79F157F3-8A67-43D3-8511-1DE9F1A4BCE2}" name="Current" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{060F2937-C4F6-498D-A578-F2C3BB45B961}" name="Capacity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -707,476 +900,921 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462D2C0A-38B0-4D44-B1EA-05D7D542B68B}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1476</v>
+      </c>
+      <c r="I2" s="17">
+        <f>AVERAGE(H2:H5)</f>
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1486</v>
+      </c>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1382</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1500</v>
+      </c>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1160</v>
+      </c>
+      <c r="I6" s="17">
+        <f>AVERAGE(H6:H9)</f>
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1080</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1216</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8">
-        <v>1382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="6">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="F9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1136</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="F10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1821</v>
+      </c>
+      <c r="I10" s="17">
+        <f>AVERAGE(H10:H13)</f>
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="F11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1693</v>
+      </c>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6">
         <v>3</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1853</v>
+      </c>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="8">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="6">
         <v>4</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="F13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1741</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1816</v>
+      </c>
+      <c r="I14" s="17">
+        <f>AVERAGE(H14:H17)</f>
+        <v>1761.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1737</v>
+      </c>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1771</v>
+      </c>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="6">
-        <v>3</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="6">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="6">
-        <v>3</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="6">
-        <v>4</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1722</v>
+      </c>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="6">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6">
         <v>1</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="8">
+        <v>377</v>
+      </c>
+      <c r="I18" s="17">
+        <f>AVERAGE(H18:H21)</f>
+        <v>377.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="6">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="6">
         <v>2</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="8">
+        <v>384</v>
+      </c>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="6">
+        <v>11</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="6">
         <v>3</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="8">
+        <v>372</v>
+      </c>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="6">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="6">
         <v>4</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="8">
+        <v>378</v>
+      </c>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="6">
         <v>1</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="6">
         <v>2</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="6">
         <v>3</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="6">
         <v>4</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="6">
+        <v>11</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="6">
+        <v>11</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="6">
         <v>2</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="6">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="6">
         <v>3</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="6">
+        <v>11</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="6">
         <v>4</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="F29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="6">
+        <v>2</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="6">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="6">
+        <v>4</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="18"/>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I26:I29"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I22:I25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>